<commit_message>
Cambio ded arch a 12b. Pendiente de simular y probar en placa
</commit_message>
<xml_diff>
--- a/MATLAB/SintesisYRecursos.xlsx
+++ b/MATLAB/SintesisYRecursos.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eros_\Downloads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="28455" windowHeight="12540"/>
   </bookViews>
@@ -22,7 +27,7 @@
     <sheet name="Timing Filter" sheetId="15" r:id="rId13"/>
     <sheet name="Timing Config_Reverb" sheetId="16" r:id="rId14"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -635,8 +640,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1107,6 +1112,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1153,7 +1166,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1185,9 +1198,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1219,6 +1233,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1394,14 +1409,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D4:Q22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="29.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.7109375" style="1" bestFit="1" customWidth="1"/>
@@ -1419,13 +1434,13 @@
     <col min="17" max="17" width="3.85546875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="4:17" ht="15.75" thickBot="1"/>
-    <row r="5" spans="4:17" ht="15.75" thickBot="1">
+    <row r="4" spans="4:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="4:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D5" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="4:17" ht="15.75" thickBot="1">
+    <row r="6" spans="4:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D6" s="5" t="s">
         <v>12</v>
       </c>
@@ -1469,7 +1484,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="7" spans="4:17">
+    <row r="7" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D7" s="12" t="s">
         <v>11</v>
       </c>
@@ -1513,7 +1528,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="4:17">
+    <row r="8" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D8" s="3" t="s">
         <v>0</v>
       </c>
@@ -1557,7 +1572,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="4:17">
+    <row r="9" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D9" s="4" t="s">
         <v>1</v>
       </c>
@@ -1601,7 +1616,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="4:17">
+    <row r="10" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D10" s="3" t="s">
         <v>2</v>
       </c>
@@ -1645,7 +1660,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="4:17">
+    <row r="11" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D11" s="4" t="s">
         <v>3</v>
       </c>
@@ -1689,7 +1704,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="4:17">
+    <row r="12" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D12" s="3" t="s">
         <v>4</v>
       </c>
@@ -1733,7 +1748,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="4:17">
+    <row r="13" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D13" s="4" t="s">
         <v>139</v>
       </c>
@@ -1777,7 +1792,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="4:17">
+    <row r="14" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D14" s="3" t="s">
         <v>5</v>
       </c>
@@ -1821,7 +1836,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="4:17">
+    <row r="15" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D15" s="4" t="s">
         <v>6</v>
       </c>
@@ -1865,7 +1880,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="4:17">
+    <row r="16" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D16" s="3" t="s">
         <v>7</v>
       </c>
@@ -1909,7 +1924,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="4:17">
+    <row r="17" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D17" s="4" t="s">
         <v>8</v>
       </c>
@@ -1953,7 +1968,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="4:17">
+    <row r="18" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D18" s="3" t="s">
         <v>9</v>
       </c>
@@ -1997,7 +2012,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="4:17" ht="15.75" thickBot="1">
+    <row r="19" spans="4:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D19" s="17" t="s">
         <v>10</v>
       </c>
@@ -2010,7 +2025,9 @@
       <c r="G19" s="26">
         <v>51.978000000000002</v>
       </c>
-      <c r="H19" s="26"/>
+      <c r="H19" s="26">
+        <v>0.22700000000000001</v>
+      </c>
       <c r="I19" s="26">
         <f>I7+I8+I9+I10+I11+I12+I13+I14+I15+I16+I17+I18</f>
         <v>12500</v>
@@ -2040,7 +2057,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="4:17" ht="15.75" thickBot="1">
+    <row r="20" spans="4:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G20" s="31">
         <f>MIN(G8,G9,G10,G11,G12,G13,G14,G15,G16,G17,G18)</f>
         <v>63.539000000000001</v>
@@ -2070,7 +2087,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="4:17">
+    <row r="22" spans="4:17" x14ac:dyDescent="0.25">
       <c r="E22" s="16"/>
     </row>
   </sheetData>
@@ -2080,14 +2097,14 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.42578125" customWidth="1"/>
     <col min="2" max="2" width="11.5703125" customWidth="1"/>
@@ -2103,7 +2120,7 @@
     <col min="14" max="14" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>22</v>
       </c>
@@ -2147,7 +2164,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>36</v>
       </c>
@@ -2191,7 +2208,7 @@
         <v>0.12928900122642517</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>41</v>
       </c>
@@ -2235,7 +2252,7 @@
         <v>0.12928900122642517</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>43</v>
       </c>
@@ -2279,7 +2296,7 @@
         <v>0.12928900122642517</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>45</v>
       </c>
@@ -2323,7 +2340,7 @@
         <v>0.12928900122642517</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>47</v>
       </c>
@@ -2367,12 +2384,12 @@
         <v>0.12928900122642517</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>49</v>
       </c>
       <c r="B7" s="14">
-        <v>74.575363159179687</v>
+        <v>74.575363159179688</v>
       </c>
       <c r="C7" s="15">
         <v>0</v>
@@ -2411,7 +2428,7 @@
         <v>0.12928900122642517</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>51</v>
       </c>
@@ -2455,7 +2472,7 @@
         <v>0.12928900122642517</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>53</v>
       </c>
@@ -2499,7 +2516,7 @@
         <v>0.12928900122642517</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>55</v>
       </c>
@@ -2543,7 +2560,7 @@
         <v>0.12928900122642517</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
         <v>57</v>
       </c>
@@ -2593,14 +2610,14 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.42578125" customWidth="1"/>
     <col min="2" max="2" width="11.5703125" customWidth="1"/>
@@ -2617,7 +2634,7 @@
     <col min="14" max="14" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>22</v>
       </c>
@@ -2661,7 +2678,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>36</v>
       </c>
@@ -2705,7 +2722,7 @@
         <v>0.12928900122642517</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>41</v>
       </c>
@@ -2749,12 +2766,12 @@
         <v>0.12928900122642517</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>43</v>
       </c>
       <c r="B4" s="14">
-        <v>79.259780883789062</v>
+        <v>79.259780883789063</v>
       </c>
       <c r="C4" s="15">
         <v>5</v>
@@ -2793,12 +2810,12 @@
         <v>0.12928900122642517</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>45</v>
       </c>
       <c r="B5" s="14">
-        <v>79.259780883789062</v>
+        <v>79.259780883789063</v>
       </c>
       <c r="C5" s="15">
         <v>5</v>
@@ -2837,7 +2854,7 @@
         <v>0.12928900122642517</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>47</v>
       </c>
@@ -2881,7 +2898,7 @@
         <v>0.12928900122642517</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>49</v>
       </c>
@@ -2925,7 +2942,7 @@
         <v>0.12928900122642517</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>51</v>
       </c>
@@ -2945,7 +2962,7 @@
         <v>68</v>
       </c>
       <c r="G8" s="14">
-        <v>8.8392410278320312</v>
+        <v>8.8392410278320313</v>
       </c>
       <c r="H8" s="14">
         <v>1.5580002069473267</v>
@@ -2969,7 +2986,7 @@
         <v>0.12928900122642517</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>53</v>
       </c>
@@ -3013,7 +3030,7 @@
         <v>0.12928900122642517</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>55</v>
       </c>
@@ -3057,7 +3074,7 @@
         <v>0.12928900122642517</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
         <v>57</v>
       </c>
@@ -3107,14 +3124,14 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.42578125" customWidth="1"/>
     <col min="2" max="2" width="11.5703125" customWidth="1"/>
@@ -3131,7 +3148,7 @@
     <col min="14" max="14" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>22</v>
       </c>
@@ -3175,7 +3192,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>36</v>
       </c>
@@ -3219,7 +3236,7 @@
         <v>0.12928900122642517</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>41</v>
       </c>
@@ -3263,7 +3280,7 @@
         <v>0.12928900122642517</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>43</v>
       </c>
@@ -3307,7 +3324,7 @@
         <v>0.12928900122642517</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>45</v>
       </c>
@@ -3351,7 +3368,7 @@
         <v>0.12928900122642517</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>47</v>
       </c>
@@ -3395,7 +3412,7 @@
         <v>0.12928900122642517</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>49</v>
       </c>
@@ -3439,7 +3456,7 @@
         <v>0.12928900122642517</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>51</v>
       </c>
@@ -3483,7 +3500,7 @@
         <v>0.12928900122642517</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>53</v>
       </c>
@@ -3527,7 +3544,7 @@
         <v>0.12928900122642517</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>55</v>
       </c>
@@ -3571,7 +3588,7 @@
         <v>0.12928900122642517</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
         <v>57</v>
       </c>
@@ -3621,14 +3638,14 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.42578125" customWidth="1"/>
     <col min="2" max="2" width="11.5703125" customWidth="1"/>
@@ -3644,7 +3661,7 @@
     <col min="14" max="14" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>22</v>
       </c>
@@ -3688,7 +3705,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>36</v>
       </c>
@@ -3732,7 +3749,7 @@
         <v>0.12928900122642517</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>41</v>
       </c>
@@ -3776,7 +3793,7 @@
         <v>0.12928900122642517</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>43</v>
       </c>
@@ -3820,7 +3837,7 @@
         <v>0.12928900122642517</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>45</v>
       </c>
@@ -3864,7 +3881,7 @@
         <v>0.12928900122642517</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>47</v>
       </c>
@@ -3908,7 +3925,7 @@
         <v>0.12928900122642517</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>49</v>
       </c>
@@ -3952,7 +3969,7 @@
         <v>0.12928900122642517</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>51</v>
       </c>
@@ -3996,7 +4013,7 @@
         <v>0.12928900122642517</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>53</v>
       </c>
@@ -4040,7 +4057,7 @@
         <v>0.12928900122642517</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>55</v>
       </c>
@@ -4084,7 +4101,7 @@
         <v>0.12928900122642517</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
         <v>57</v>
       </c>
@@ -4134,14 +4151,14 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.42578125" customWidth="1"/>
     <col min="2" max="2" width="11.5703125" customWidth="1"/>
@@ -4157,7 +4174,7 @@
     <col min="14" max="14" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>22</v>
       </c>
@@ -4201,7 +4218,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>36</v>
       </c>
@@ -4245,7 +4262,7 @@
         <v>0.12928900122642517</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>41</v>
       </c>
@@ -4289,7 +4306,7 @@
         <v>0.12928900122642517</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>43</v>
       </c>
@@ -4333,7 +4350,7 @@
         <v>0.12928900122642517</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>45</v>
       </c>
@@ -4377,7 +4394,7 @@
         <v>0.12928900122642517</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>47</v>
       </c>
@@ -4421,7 +4438,7 @@
         <v>0.12928900122642517</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>49</v>
       </c>
@@ -4465,7 +4482,7 @@
         <v>0.12928900122642517</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>51</v>
       </c>
@@ -4509,7 +4526,7 @@
         <v>0.12928900122642517</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>53</v>
       </c>
@@ -4553,7 +4570,7 @@
         <v>0.12928900122642517</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>55</v>
       </c>
@@ -4597,7 +4614,7 @@
         <v>0.12928900122642517</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
         <v>57</v>
       </c>
@@ -4647,14 +4664,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.42578125" customWidth="1"/>
     <col min="2" max="2" width="11.5703125" customWidth="1"/>
@@ -4671,7 +4688,7 @@
     <col min="14" max="14" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>22</v>
       </c>
@@ -4715,12 +4732,12 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>36</v>
       </c>
       <c r="B2" s="14">
-        <v>51.978317260742187</v>
+        <v>51.978317260742188</v>
       </c>
       <c r="C2" s="15">
         <v>5</v>
@@ -4759,12 +4776,12 @@
         <v>0.12928900122642517</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>41</v>
       </c>
       <c r="B3" s="14">
-        <v>51.978317260742187</v>
+        <v>51.978317260742188</v>
       </c>
       <c r="C3" s="15">
         <v>5</v>
@@ -4803,12 +4820,12 @@
         <v>0.12928900122642517</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>43</v>
       </c>
       <c r="B4" s="14">
-        <v>51.978317260742187</v>
+        <v>51.978317260742188</v>
       </c>
       <c r="C4" s="15">
         <v>5</v>
@@ -4847,12 +4864,12 @@
         <v>0.12928900122642517</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>45</v>
       </c>
       <c r="B5" s="14">
-        <v>51.978317260742187</v>
+        <v>51.978317260742188</v>
       </c>
       <c r="C5" s="15">
         <v>5</v>
@@ -4891,7 +4908,7 @@
         <v>0.12928900122642517</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>47</v>
       </c>
@@ -4935,7 +4952,7 @@
         <v>0.12928900122642517</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>49</v>
       </c>
@@ -4979,7 +4996,7 @@
         <v>0.12928900122642517</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>51</v>
       </c>
@@ -5023,7 +5040,7 @@
         <v>0.12928900122642517</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>53</v>
       </c>
@@ -5067,7 +5084,7 @@
         <v>0.12928900122642517</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>55</v>
       </c>
@@ -5111,7 +5128,7 @@
         <v>0.12928900122642517</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
         <v>57</v>
       </c>
@@ -5161,14 +5178,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.42578125" customWidth="1"/>
     <col min="2" max="2" width="11.5703125" customWidth="1"/>
@@ -5185,7 +5202,7 @@
     <col min="14" max="14" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>22</v>
       </c>
@@ -5229,7 +5246,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>36</v>
       </c>
@@ -5273,7 +5290,7 @@
         <v>0.12928900122642517</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>41</v>
       </c>
@@ -5317,7 +5334,7 @@
         <v>0.12928900122642517</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>43</v>
       </c>
@@ -5361,7 +5378,7 @@
         <v>0.12928900122642517</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>45</v>
       </c>
@@ -5405,12 +5422,12 @@
         <v>0.12928900122642517</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>47</v>
       </c>
       <c r="B6" s="14">
-        <v>77.403366088867187</v>
+        <v>77.403366088867188</v>
       </c>
       <c r="C6" s="15">
         <v>7</v>
@@ -5449,7 +5466,7 @@
         <v>0.12928900122642517</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>49</v>
       </c>
@@ -5493,7 +5510,7 @@
         <v>0.12928900122642517</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>51</v>
       </c>
@@ -5537,7 +5554,7 @@
         <v>0.12928900122642517</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>53</v>
       </c>
@@ -5581,7 +5598,7 @@
         <v>0.12928900122642517</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>55</v>
       </c>
@@ -5625,7 +5642,7 @@
         <v>0.12928900122642517</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
         <v>57</v>
       </c>
@@ -5675,14 +5692,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.42578125" customWidth="1"/>
     <col min="2" max="2" width="11.5703125" customWidth="1"/>
@@ -5699,7 +5716,7 @@
     <col min="14" max="14" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>22</v>
       </c>
@@ -5743,7 +5760,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>36</v>
       </c>
@@ -5787,7 +5804,7 @@
         <v>0.12928900122642517</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>41</v>
       </c>
@@ -5831,7 +5848,7 @@
         <v>0.12928900122642517</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>43</v>
       </c>
@@ -5875,7 +5892,7 @@
         <v>0.12928900122642517</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>45</v>
       </c>
@@ -5919,7 +5936,7 @@
         <v>0.12928900122642517</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>47</v>
       </c>
@@ -5963,7 +5980,7 @@
         <v>0.12928900122642517</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>49</v>
       </c>
@@ -5983,7 +6000,7 @@
         <v>83</v>
       </c>
       <c r="G7" s="14">
-        <v>7.7412948608398437</v>
+        <v>7.7412948608398438</v>
       </c>
       <c r="H7" s="14">
         <v>1.7979999780654907</v>
@@ -6007,7 +6024,7 @@
         <v>0.12928900122642517</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>51</v>
       </c>
@@ -6027,7 +6044,7 @@
         <v>75</v>
       </c>
       <c r="G8" s="14">
-        <v>7.7412948608398437</v>
+        <v>7.7412948608398438</v>
       </c>
       <c r="H8" s="14">
         <v>1.7979999780654907</v>
@@ -6051,7 +6068,7 @@
         <v>0.12928900122642517</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>53</v>
       </c>
@@ -6095,7 +6112,7 @@
         <v>0.12928900122642517</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>55</v>
       </c>
@@ -6139,7 +6156,7 @@
         <v>0.12928900122642517</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
         <v>57</v>
       </c>
@@ -6189,14 +6206,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.42578125" customWidth="1"/>
     <col min="2" max="2" width="11.5703125" customWidth="1"/>
@@ -6213,7 +6230,7 @@
     <col min="14" max="14" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>22</v>
       </c>
@@ -6257,7 +6274,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>36</v>
       </c>
@@ -6301,7 +6318,7 @@
         <v>0.12928900122642517</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>41</v>
       </c>
@@ -6345,7 +6362,7 @@
         <v>0.12928900122642517</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>43</v>
       </c>
@@ -6389,7 +6406,7 @@
         <v>0.12928900122642517</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>45</v>
       </c>
@@ -6433,7 +6450,7 @@
         <v>0.12928900122642517</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>47</v>
       </c>
@@ -6477,7 +6494,7 @@
         <v>0.12928900122642517</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>49</v>
       </c>
@@ -6521,7 +6538,7 @@
         <v>0.12928900122642517</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>51</v>
       </c>
@@ -6565,7 +6582,7 @@
         <v>0.12928900122642517</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>53</v>
       </c>
@@ -6609,7 +6626,7 @@
         <v>0.12928900122642517</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>55</v>
       </c>
@@ -6653,7 +6670,7 @@
         <v>0.12928900122642517</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
         <v>57</v>
       </c>
@@ -6703,14 +6720,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.5703125" bestFit="1" customWidth="1"/>
@@ -6726,7 +6743,7 @@
     <col min="14" max="14" width="16.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>22</v>
       </c>
@@ -6770,7 +6787,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>36</v>
       </c>
@@ -6814,7 +6831,7 @@
         <v>0.12928900122642517</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>41</v>
       </c>
@@ -6858,7 +6875,7 @@
         <v>0.12928900122642517</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>43</v>
       </c>
@@ -6902,7 +6919,7 @@
         <v>0.12928900122642517</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>45</v>
       </c>
@@ -6946,7 +6963,7 @@
         <v>0.12928900122642517</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>47</v>
       </c>
@@ -6966,7 +6983,7 @@
         <v>105</v>
       </c>
       <c r="G6" s="14">
-        <v>24.074508666992187</v>
+        <v>24.074508666992188</v>
       </c>
       <c r="H6" s="14">
         <v>2.5899999141693115</v>
@@ -6990,7 +7007,7 @@
         <v>0.12928900122642517</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>49</v>
       </c>
@@ -7034,7 +7051,7 @@
         <v>0.12928900122642517</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>51</v>
       </c>
@@ -7078,7 +7095,7 @@
         <v>0.12928900122642517</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>53</v>
       </c>
@@ -7122,7 +7139,7 @@
         <v>0.12928900122642517</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>55</v>
       </c>
@@ -7166,7 +7183,7 @@
         <v>0.12928900122642517</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
         <v>57</v>
       </c>
@@ -7216,14 +7233,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.42578125" customWidth="1"/>
     <col min="2" max="2" width="11.5703125" customWidth="1"/>
@@ -7240,7 +7257,7 @@
     <col min="14" max="14" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>22</v>
       </c>
@@ -7284,7 +7301,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>36</v>
       </c>
@@ -7328,7 +7345,7 @@
         <v>0.12928900122642517</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>41</v>
       </c>
@@ -7372,7 +7389,7 @@
         <v>0.12928900122642517</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>43</v>
       </c>
@@ -7416,7 +7433,7 @@
         <v>0.12928900122642517</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>45</v>
       </c>
@@ -7460,7 +7477,7 @@
         <v>0.12928900122642517</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>47</v>
       </c>
@@ -7504,7 +7521,7 @@
         <v>0.12928900122642517</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>49</v>
       </c>
@@ -7548,7 +7565,7 @@
         <v>0.12928900122642517</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>51</v>
       </c>
@@ -7592,7 +7609,7 @@
         <v>0.12928900122642517</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>53</v>
       </c>
@@ -7636,7 +7653,7 @@
         <v>0.12928900122642517</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>55</v>
       </c>
@@ -7680,7 +7697,7 @@
         <v>0.12928900122642517</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
         <v>57</v>
       </c>
@@ -7730,14 +7747,14 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.42578125" customWidth="1"/>
     <col min="2" max="2" width="11.5703125" customWidth="1"/>
@@ -7753,7 +7770,7 @@
     <col min="14" max="14" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>22</v>
       </c>
@@ -7797,7 +7814,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>36</v>
       </c>
@@ -7841,7 +7858,7 @@
         <v>0.12928900122642517</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>41</v>
       </c>
@@ -7885,7 +7902,7 @@
         <v>0.12928900122642517</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>43</v>
       </c>
@@ -7929,7 +7946,7 @@
         <v>0.12928900122642517</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>45</v>
       </c>
@@ -7973,7 +7990,7 @@
         <v>0.12928900122642517</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>47</v>
       </c>
@@ -8017,7 +8034,7 @@
         <v>0.12928900122642517</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>49</v>
       </c>
@@ -8061,7 +8078,7 @@
         <v>0.12928900122642517</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>51</v>
       </c>
@@ -8105,7 +8122,7 @@
         <v>0.12928900122642517</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>53</v>
       </c>
@@ -8149,7 +8166,7 @@
         <v>0.12928900122642517</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>55</v>
       </c>
@@ -8193,7 +8210,7 @@
         <v>0.12928900122642517</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
         <v>57</v>
       </c>
@@ -8243,14 +8260,14 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.42578125" customWidth="1"/>
     <col min="2" max="2" width="11.5703125" customWidth="1"/>
@@ -8266,7 +8283,7 @@
     <col min="14" max="14" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>22</v>
       </c>
@@ -8310,7 +8327,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>36</v>
       </c>
@@ -8354,7 +8371,7 @@
         <v>0.12928900122642517</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>41</v>
       </c>
@@ -8398,7 +8415,7 @@
         <v>0.12928900122642517</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>43</v>
       </c>
@@ -8442,7 +8459,7 @@
         <v>0.12928900122642517</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>45</v>
       </c>
@@ -8486,7 +8503,7 @@
         <v>0.12928900122642517</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>47</v>
       </c>
@@ -8530,7 +8547,7 @@
         <v>0.12928900122642517</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>49</v>
       </c>
@@ -8574,7 +8591,7 @@
         <v>0.12928900122642517</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>51</v>
       </c>
@@ -8618,7 +8635,7 @@
         <v>0.12928900122642517</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>53</v>
       </c>
@@ -8662,7 +8679,7 @@
         <v>0.12928900122642517</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>55</v>
       </c>
@@ -8706,7 +8723,7 @@
         <v>0.12928900122642517</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
         <v>57</v>
       </c>

</xml_diff>

<commit_message>
Estudio del ECO con distintas N. Pendiente hacer las gráficas
</commit_message>
<xml_diff>
--- a/MATLAB/SintesisYRecursos.xlsx
+++ b/MATLAB/SintesisYRecursos.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1016" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1049" uniqueCount="219">
   <si>
     <t>ES</t>
   </si>
@@ -630,6 +630,60 @@
   </si>
   <si>
     <t>59s</t>
+  </si>
+  <si>
+    <t>ECO\Recursos para 16b</t>
+  </si>
+  <si>
+    <t>1m 56s</t>
+  </si>
+  <si>
+    <t>56s</t>
+  </si>
+  <si>
+    <t>54m 01s</t>
+  </si>
+  <si>
+    <t>2m 03s</t>
+  </si>
+  <si>
+    <t>30m 04s</t>
+  </si>
+  <si>
+    <t>1m 40s</t>
+  </si>
+  <si>
+    <t>20m 59s</t>
+  </si>
+  <si>
+    <t>1m 29s</t>
+  </si>
+  <si>
+    <t>13m 14s</t>
+  </si>
+  <si>
+    <t>1m 23s</t>
+  </si>
+  <si>
+    <t>9m 44s</t>
+  </si>
+  <si>
+    <t>1m 14s</t>
+  </si>
+  <si>
+    <t>5m 53s</t>
+  </si>
+  <si>
+    <t>1m 08s</t>
+  </si>
+  <si>
+    <t>3m 22s</t>
+  </si>
+  <si>
+    <t>1m 02s</t>
+  </si>
+  <si>
+    <t>2m 16s</t>
   </si>
 </sst>
 </file>
@@ -690,7 +744,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -999,11 +1053,74 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1099,6 +1216,33 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1395,10 +1539,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="D4:Q22"/>
+  <dimension ref="D4:Q33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1734,46 +1878,46 @@
       </c>
     </row>
     <row r="13" spans="4:17">
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="33" t="s">
         <v>139</v>
       </c>
       <c r="E13" s="32" t="s">
         <v>167</v>
       </c>
-      <c r="F13" s="6" t="s">
+      <c r="F13" s="34" t="s">
         <v>168</v>
       </c>
-      <c r="G13" s="6">
+      <c r="G13" s="34">
         <v>63.539000000000001</v>
       </c>
-      <c r="H13" s="6">
+      <c r="H13" s="34">
         <v>0.215</v>
       </c>
-      <c r="I13" s="6">
+      <c r="I13" s="34">
         <v>5000</v>
       </c>
-      <c r="J13" s="6">
+      <c r="J13" s="34">
         <v>10344</v>
       </c>
-      <c r="K13" s="6">
+      <c r="K13" s="34">
         <v>9734</v>
       </c>
-      <c r="L13" s="6">
+      <c r="L13" s="34">
         <v>5337</v>
       </c>
-      <c r="M13" s="6">
+      <c r="M13" s="34">
         <v>0</v>
       </c>
-      <c r="N13" s="6">
+      <c r="N13" s="34">
         <v>0</v>
       </c>
-      <c r="O13" s="6">
+      <c r="O13" s="34">
         <v>55</v>
       </c>
-      <c r="P13" s="6">
+      <c r="P13" s="34">
         <v>2</v>
       </c>
-      <c r="Q13" s="24">
+      <c r="Q13" s="35">
         <v>1</v>
       </c>
     </row>
@@ -2070,8 +2214,453 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="4:17">
+    <row r="22" spans="4:17" ht="15.75" thickBot="1">
       <c r="E22" s="16"/>
+    </row>
+    <row r="23" spans="4:17" ht="15.75" thickBot="1">
+      <c r="D23" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="4:17" ht="15.75" thickBot="1">
+      <c r="D24" s="36" t="s">
+        <v>201</v>
+      </c>
+      <c r="E24" s="37" t="s">
+        <v>13</v>
+      </c>
+      <c r="F24" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G24" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="H24" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="I24" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="J24" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="K24" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="L24" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="M24" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="N24" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="O24" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="P24" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q24" s="11" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="25" spans="4:17">
+      <c r="D25" s="38">
+        <v>500</v>
+      </c>
+      <c r="E25" s="39" t="s">
+        <v>202</v>
+      </c>
+      <c r="F25" s="40" t="s">
+        <v>203</v>
+      </c>
+      <c r="G25" s="40">
+        <v>74.114999999999995</v>
+      </c>
+      <c r="H25" s="40">
+        <v>0.21299999999999999</v>
+      </c>
+      <c r="I25" s="40">
+        <v>500</v>
+      </c>
+      <c r="J25" s="40">
+        <v>1549</v>
+      </c>
+      <c r="K25" s="40">
+        <v>992</v>
+      </c>
+      <c r="L25" s="40">
+        <v>837</v>
+      </c>
+      <c r="M25" s="40">
+        <v>0</v>
+      </c>
+      <c r="N25" s="40">
+        <v>0</v>
+      </c>
+      <c r="O25" s="40">
+        <v>55</v>
+      </c>
+      <c r="P25" s="40">
+        <v>2</v>
+      </c>
+      <c r="Q25" s="40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="4:17">
+      <c r="D26" s="4">
+        <v>750</v>
+      </c>
+      <c r="E26" s="41" t="s">
+        <v>218</v>
+      </c>
+      <c r="F26" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="G26" s="6">
+        <v>69.844999999999999</v>
+      </c>
+      <c r="H26" s="6">
+        <v>0.21299999999999999</v>
+      </c>
+      <c r="I26" s="6">
+        <v>1000</v>
+      </c>
+      <c r="J26" s="6">
+        <v>2132</v>
+      </c>
+      <c r="K26" s="6">
+        <v>1536</v>
+      </c>
+      <c r="L26" s="6">
+        <v>1091</v>
+      </c>
+      <c r="M26" s="6">
+        <v>0</v>
+      </c>
+      <c r="N26" s="6">
+        <v>0</v>
+      </c>
+      <c r="O26" s="6">
+        <v>55</v>
+      </c>
+      <c r="P26" s="6">
+        <v>2</v>
+      </c>
+      <c r="Q26" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="4:17">
+      <c r="D27" s="4">
+        <v>1000</v>
+      </c>
+      <c r="E27" s="41" t="s">
+        <v>216</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="G27" s="6">
+        <v>69.037999999999997</v>
+      </c>
+      <c r="H27" s="6">
+        <v>0.21299999999999999</v>
+      </c>
+      <c r="I27" s="6">
+        <v>1000</v>
+      </c>
+      <c r="J27" s="6">
+        <v>2643</v>
+      </c>
+      <c r="K27" s="6">
+        <v>2048</v>
+      </c>
+      <c r="L27" s="6">
+        <v>1341</v>
+      </c>
+      <c r="M27" s="6">
+        <v>0</v>
+      </c>
+      <c r="N27" s="6">
+        <v>0</v>
+      </c>
+      <c r="O27" s="6">
+        <v>55</v>
+      </c>
+      <c r="P27" s="6">
+        <v>2</v>
+      </c>
+      <c r="Q27" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="4:17">
+      <c r="D28" s="4">
+        <v>1500</v>
+      </c>
+      <c r="E28" s="41" t="s">
+        <v>214</v>
+      </c>
+      <c r="F28" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="G28" s="6">
+        <v>68.638999999999996</v>
+      </c>
+      <c r="H28" s="6">
+        <v>0.21299999999999999</v>
+      </c>
+      <c r="I28" s="6">
+        <v>1500</v>
+      </c>
+      <c r="J28" s="6">
+        <v>3703</v>
+      </c>
+      <c r="K28" s="6">
+        <v>3102</v>
+      </c>
+      <c r="L28" s="6">
+        <v>1845</v>
+      </c>
+      <c r="M28" s="6">
+        <v>0</v>
+      </c>
+      <c r="N28" s="6">
+        <v>0</v>
+      </c>
+      <c r="O28" s="6">
+        <v>55</v>
+      </c>
+      <c r="P28" s="6">
+        <v>2</v>
+      </c>
+      <c r="Q28" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="4:17">
+      <c r="D29" s="4">
+        <v>2000</v>
+      </c>
+      <c r="E29" s="41" t="s">
+        <v>212</v>
+      </c>
+      <c r="F29" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="G29" s="6">
+        <v>64.658000000000001</v>
+      </c>
+      <c r="H29" s="6">
+        <v>0.214</v>
+      </c>
+      <c r="I29" s="6">
+        <v>2000</v>
+      </c>
+      <c r="J29" s="6">
+        <v>4753</v>
+      </c>
+      <c r="K29" s="6">
+        <v>4158</v>
+      </c>
+      <c r="L29" s="6">
+        <v>2345</v>
+      </c>
+      <c r="M29" s="6">
+        <v>0</v>
+      </c>
+      <c r="N29" s="6">
+        <v>0</v>
+      </c>
+      <c r="O29" s="6">
+        <v>55</v>
+      </c>
+      <c r="P29" s="6">
+        <v>2</v>
+      </c>
+      <c r="Q29" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="4:17">
+      <c r="D30" s="4">
+        <v>2750</v>
+      </c>
+      <c r="E30" s="41" t="s">
+        <v>210</v>
+      </c>
+      <c r="F30" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="G30" s="6">
+        <v>62.606999999999999</v>
+      </c>
+      <c r="H30" s="6">
+        <v>0.214</v>
+      </c>
+      <c r="I30" s="6">
+        <v>2750</v>
+      </c>
+      <c r="J30" s="6">
+        <v>5940</v>
+      </c>
+      <c r="K30" s="6">
+        <v>5332</v>
+      </c>
+      <c r="L30" s="6">
+        <v>3087</v>
+      </c>
+      <c r="M30" s="6">
+        <v>0</v>
+      </c>
+      <c r="N30" s="6">
+        <v>0</v>
+      </c>
+      <c r="O30" s="6">
+        <v>55</v>
+      </c>
+      <c r="P30" s="6">
+        <v>2</v>
+      </c>
+      <c r="Q30" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="4:17">
+      <c r="D31" s="4">
+        <v>3500</v>
+      </c>
+      <c r="E31" s="41" t="s">
+        <v>208</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="G31" s="6">
+        <v>61.154000000000003</v>
+      </c>
+      <c r="H31" s="6">
+        <v>0.214</v>
+      </c>
+      <c r="I31" s="6">
+        <v>3500</v>
+      </c>
+      <c r="J31" s="6">
+        <v>7429</v>
+      </c>
+      <c r="K31" s="6">
+        <v>6820</v>
+      </c>
+      <c r="L31" s="6">
+        <v>3837</v>
+      </c>
+      <c r="M31" s="6">
+        <v>0</v>
+      </c>
+      <c r="N31" s="6">
+        <v>0</v>
+      </c>
+      <c r="O31" s="6">
+        <v>55</v>
+      </c>
+      <c r="P31" s="6">
+        <v>2</v>
+      </c>
+      <c r="Q31" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="4:17">
+      <c r="D32" s="4">
+        <v>4500</v>
+      </c>
+      <c r="E32" s="41" t="s">
+        <v>206</v>
+      </c>
+      <c r="F32" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="G32" s="6">
+        <v>65.067999999999998</v>
+      </c>
+      <c r="H32" s="6">
+        <v>0.215</v>
+      </c>
+      <c r="I32" s="6">
+        <v>4500</v>
+      </c>
+      <c r="J32" s="6">
+        <v>9353</v>
+      </c>
+      <c r="K32" s="6">
+        <v>8742</v>
+      </c>
+      <c r="L32" s="6">
+        <v>4837</v>
+      </c>
+      <c r="M32" s="6">
+        <v>0</v>
+      </c>
+      <c r="N32" s="6">
+        <v>0</v>
+      </c>
+      <c r="O32" s="6">
+        <v>55</v>
+      </c>
+      <c r="P32" s="6">
+        <v>2</v>
+      </c>
+      <c r="Q32" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="4:17" ht="15.75" thickBot="1">
+      <c r="D33" s="17">
+        <v>6000</v>
+      </c>
+      <c r="E33" s="41" t="s">
+        <v>204</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="G33" s="6">
+        <v>60.475000000000001</v>
+      </c>
+      <c r="H33" s="6">
+        <v>0.215</v>
+      </c>
+      <c r="I33" s="6">
+        <v>6000</v>
+      </c>
+      <c r="J33" s="6">
+        <v>12264</v>
+      </c>
+      <c r="K33" s="6">
+        <v>11656</v>
+      </c>
+      <c r="L33" s="6">
+        <v>6337</v>
+      </c>
+      <c r="M33" s="6">
+        <v>0</v>
+      </c>
+      <c r="N33" s="6">
+        <v>0</v>
+      </c>
+      <c r="O33" s="6">
+        <v>55</v>
+      </c>
+      <c r="P33" s="6">
+        <v>2</v>
+      </c>
+      <c r="Q33" s="6">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>